<commit_message>
send 30 01 2023
</commit_message>
<xml_diff>
--- a/Exercices Merise/Bobliotheque/dependance fonctionnelle.xlsx
+++ b/Exercices Merise/Bobliotheque/dependance fonctionnelle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grognone\Desktop\SaveCdaJay\SavecdaJay\Exercices Merise\Bobliotheque\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B30754E-D8E6-4D72-A881-6311F2666ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1050599-0F4E-4B9C-884A-19E0C68F8C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="3270" windowWidth="21600" windowHeight="11385" xr2:uid="{FD19F1B3-1EE5-45CE-8C09-71ACADD02B0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD19F1B3-1EE5-45CE-8C09-71ACADD02B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>Colonne1</t>
-  </si>
-  <si>
-    <t>Colonne2</t>
   </si>
   <si>
     <t>Colonne3</t>
@@ -209,11 +206,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8E2A03F-1F5B-41F9-9290-972E176F8DF7}" name="Tableau1" displayName="Tableau1" ref="A1:G25" totalsRowShown="0">
-  <autoFilter ref="A1:G25" xr:uid="{B8E2A03F-1F5B-41F9-9290-972E176F8DF7}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B8E2A03F-1F5B-41F9-9290-972E176F8DF7}" name="Tableau1" displayName="Tableau1" ref="A1:F25" totalsRowShown="0">
+  <autoFilter ref="A1:F25" xr:uid="{B8E2A03F-1F5B-41F9-9290-972E176F8DF7}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{FFA69651-CBD6-487D-AA29-8E29C5966ED8}" name="Colonne1"/>
-    <tableColumn id="2" xr3:uid="{F97CE35D-AA1B-4A00-929A-3503CA44EAF8}" name="Colonne2"/>
     <tableColumn id="3" xr3:uid="{80580DC3-6BCC-459C-B7BA-4C6BE4C6E388}" name="Colonne3"/>
     <tableColumn id="4" xr3:uid="{8E78722B-38E4-4581-BD6F-6CF068DB7023}" name="Colonne4"/>
     <tableColumn id="5" xr3:uid="{ADE29885-E5AD-4F54-88D4-366001ED2216}" name="Colonne5"/>
@@ -521,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092DCC80-2570-41C9-A557-35EB2A007002}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +531,7 @@
     <col min="5" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -554,209 +550,200 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25">
+      <c r="F25">
         <v>1</v>
       </c>
     </row>
@@ -788,29 +775,29 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -818,12 +805,12 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -831,7 +818,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -839,7 +826,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -847,7 +834,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -858,7 +845,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -866,7 +853,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -874,7 +861,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -882,7 +869,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -890,7 +877,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -898,7 +885,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -906,12 +893,12 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -919,7 +906,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -927,12 +914,12 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -940,7 +927,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -948,7 +935,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -956,7 +943,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -964,7 +951,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23">
         <v>1</v>

</xml_diff>